<commit_message>
Todo corregido a la fecha
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/BDatos.xlsx
+++ b/OYM/_DocumentosComunes/BDatos.xlsx
@@ -1105,7 +1105,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1231,10 +1231,22 @@
       <c r="C3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="6"/>
+      <c r="D3" s="6">
+        <f t="shared" ref="D3:D66" si="0">IF((N3)&gt;=50,10,"")</f>
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E66" si="1">IF((N3)&gt;=50,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F66" si="2">IF((N3)&gt;=50,20,"")</f>
+        <v>20</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G66" si="3">IF((N3)&gt;=51,IF((N3-50)&gt;50,50,IF((N3-50)&lt;0,0,(N3-50))), "" )</f>
+        <v>21</v>
+      </c>
       <c r="H3">
         <v>17</v>
       </c>
@@ -1248,7 +1260,7 @@
         <v>40</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N66" si="0">IF((H3+J3+L3+M3+O3)&lt;70,IF((H3+J3+L3+M3+O3)&gt;64,70,(H3+J3+L3+M3+O3)),(H3+J3+L3+M3+O3))</f>
+        <f t="shared" ref="N3:N66" si="4">IF((H3+J3+L3+M3+O3)&lt;70,IF((H3+J3+L3+M3+O3)&gt;64,70,(H3+J3+L3+M3+O3)),(H3+J3+L3+M3+O3))</f>
         <v>71</v>
       </c>
     </row>
@@ -1262,12 +1274,27 @@
       <c r="C4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="6"/>
+      <c r="D4" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
       <c r="H4">
         <v>20</v>
+      </c>
+      <c r="J4">
+        <v>17</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1276,8 +1303,8 @@
         <v>40</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
-        <v>60</v>
+        <f t="shared" si="4"/>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1290,15 +1317,27 @@
       <c r="C5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="6"/>
+      <c r="D5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G5" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1312,15 +1351,27 @@
       <c r="C6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G6" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1334,15 +1385,27 @@
       <c r="C7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="6"/>
+      <c r="D7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G7" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1356,10 +1419,22 @@
       <c r="C8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="6"/>
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
       <c r="H8">
         <v>19</v>
       </c>
@@ -1373,7 +1448,7 @@
         <v>30</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
     </row>
@@ -1387,10 +1462,22 @@
       <c r="C9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="6"/>
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="J9">
         <v>12</v>
       </c>
@@ -1401,7 +1488,7 @@
         <v>40</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
     </row>
@@ -1415,10 +1502,22 @@
       <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="6"/>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H10">
         <v>18</v>
       </c>
@@ -1432,7 +1531,7 @@
         <v>35</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -1446,10 +1545,22 @@
       <c r="C11" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
       <c r="H11">
         <v>15</v>
       </c>
@@ -1463,7 +1574,7 @@
         <v>40</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
     </row>
@@ -1477,10 +1588,22 @@
       <c r="C12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="6"/>
+      <c r="D12" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J12">
         <v>8</v>
       </c>
@@ -1491,7 +1614,7 @@
         <v>40</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -1505,15 +1628,27 @@
       <c r="C13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="6"/>
+      <c r="D13" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G13" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1527,10 +1662,22 @@
       <c r="C14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="6"/>
+      <c r="D14" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G14" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J14">
         <v>14</v>
       </c>
@@ -1538,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
@@ -1552,15 +1699,27 @@
       <c r="C15" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="6"/>
+      <c r="D15" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G15" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1574,10 +1733,22 @@
       <c r="C16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
       <c r="H16">
         <v>16</v>
       </c>
@@ -1591,7 +1762,7 @@
         <v>40</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
     </row>
@@ -1605,10 +1776,22 @@
       <c r="C17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="6"/>
+      <c r="D17" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G17" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J17">
         <v>14</v>
       </c>
@@ -1619,7 +1802,7 @@
         <v>35</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>49</v>
       </c>
     </row>
@@ -1633,10 +1816,22 @@
       <c r="C18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="6"/>
+      <c r="D18" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="J18">
         <v>12</v>
       </c>
@@ -1647,7 +1842,7 @@
         <v>40</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
     </row>
@@ -1661,15 +1856,27 @@
       <c r="C19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="6"/>
+      <c r="D19" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G19" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1683,10 +1890,22 @@
       <c r="C20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="6"/>
+      <c r="D20" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H20">
         <v>17</v>
       </c>
@@ -1700,7 +1919,7 @@
         <v>40</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -1714,10 +1933,22 @@
       <c r="C21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="6"/>
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
       <c r="J21">
         <v>18</v>
       </c>
@@ -1728,7 +1959,7 @@
         <v>35</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>53</v>
       </c>
     </row>
@@ -1742,10 +1973,22 @@
       <c r="C22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="6"/>
+      <c r="D22" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G22" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="H22">
         <v>18</v>
       </c>
@@ -1753,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
     </row>
@@ -1767,15 +2010,27 @@
       <c r="C23" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="6"/>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G23" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1789,10 +2044,22 @@
       <c r="C24" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="6"/>
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
       <c r="H24">
         <v>17</v>
       </c>
@@ -1806,7 +2073,7 @@
         <v>40</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>71</v>
       </c>
     </row>
@@ -1820,10 +2087,22 @@
       <c r="C25" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="6"/>
+      <c r="D25" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
       <c r="H25">
         <v>16</v>
       </c>
@@ -1837,7 +2116,7 @@
         <v>40</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
     </row>
@@ -1851,15 +2130,27 @@
       <c r="C26" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="6"/>
+      <c r="D26" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F26" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G26" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K26">
         <v>1</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1873,10 +2164,22 @@
       <c r="C27" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="6"/>
+      <c r="D27" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G27" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H27">
         <v>20</v>
       </c>
@@ -1890,7 +2193,7 @@
         <v>35</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -1904,10 +2207,22 @@
       <c r="C28" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="6"/>
+      <c r="D28" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G28" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H28">
         <v>17</v>
       </c>
@@ -1921,7 +2236,7 @@
         <v>35</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -1935,10 +2250,22 @@
       <c r="C29" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="6"/>
+      <c r="D29" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G29" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H29">
         <v>15</v>
       </c>
@@ -1952,7 +2279,7 @@
         <v>40</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -1966,19 +2293,34 @@
       <c r="C30" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="6"/>
+      <c r="D30" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E30" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F30" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G30" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J30">
         <v>8</v>
       </c>
       <c r="K30">
         <v>1</v>
       </c>
+      <c r="L30">
+        <v>25</v>
+      </c>
       <c r="N30">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,10 +2333,22 @@
       <c r="C31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="6"/>
+      <c r="D31" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E31" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F31" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G31" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J31">
         <v>12</v>
       </c>
@@ -2005,7 +2359,7 @@
         <v>20</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
@@ -2019,10 +2373,22 @@
       <c r="C32" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="6"/>
+      <c r="D32" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G32" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="H32">
         <v>19</v>
       </c>
@@ -2036,7 +2402,7 @@
         <v>20</v>
       </c>
       <c r="N32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
     </row>
@@ -2050,10 +2416,22 @@
       <c r="C33" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="6"/>
+      <c r="D33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F33" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G33" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J33">
         <v>8</v>
       </c>
@@ -2064,7 +2442,7 @@
         <v>40</v>
       </c>
       <c r="N33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -2078,10 +2456,22 @@
       <c r="C34" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="6"/>
+      <c r="D34" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F34" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G34" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="H34">
         <v>16</v>
       </c>
@@ -2095,7 +2485,7 @@
         <v>20</v>
       </c>
       <c r="N34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -2109,15 +2499,27 @@
       <c r="C35" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="6"/>
+      <c r="D35" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G35" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="N35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2131,10 +2533,22 @@
       <c r="C36" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="6"/>
+      <c r="D36" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G36" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
       <c r="H36">
         <v>16</v>
       </c>
@@ -2144,9 +2558,12 @@
       <c r="K36">
         <v>1</v>
       </c>
+      <c r="L36">
+        <v>40</v>
+      </c>
       <c r="N36">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f t="shared" si="4"/>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2159,10 +2576,22 @@
       <c r="C37" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="6"/>
+      <c r="D37" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G37" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
       <c r="H37">
         <v>18</v>
       </c>
@@ -2176,7 +2605,7 @@
         <v>20</v>
       </c>
       <c r="N37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
     </row>
@@ -2190,10 +2619,22 @@
       <c r="C38" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="6"/>
+      <c r="D38" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G38" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J38">
         <v>10</v>
       </c>
@@ -2204,7 +2645,7 @@
         <v>40</v>
       </c>
       <c r="N38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
     </row>
@@ -2218,10 +2659,22 @@
       <c r="C39" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="6"/>
+      <c r="D39" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G39" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
       <c r="H39">
         <v>19</v>
       </c>
@@ -2235,7 +2688,7 @@
         <v>40</v>
       </c>
       <c r="N39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
     </row>
@@ -2249,10 +2702,22 @@
       <c r="C40" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="6"/>
+      <c r="D40" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F40" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G40" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J40">
         <v>20</v>
       </c>
@@ -2263,7 +2728,7 @@
         <v>20</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
     </row>
@@ -2277,10 +2742,22 @@
       <c r="C41" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="6"/>
+      <c r="D41" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F41" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G41" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H41">
         <v>14</v>
       </c>
@@ -2294,7 +2771,7 @@
         <v>40</v>
       </c>
       <c r="N41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2308,10 +2785,22 @@
       <c r="C42" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="6"/>
+      <c r="D42" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E42" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F42" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G42" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H42">
         <v>17</v>
       </c>
@@ -2325,7 +2814,7 @@
         <v>40</v>
       </c>
       <c r="N42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2339,13 +2828,28 @@
       <c r="C43" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="6"/>
+      <c r="D43" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G43" s="6">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
       <c r="H43">
         <v>18</v>
       </c>
+      <c r="J43">
+        <v>16</v>
+      </c>
       <c r="K43">
         <v>1</v>
       </c>
@@ -2353,8 +2857,8 @@
         <v>40</v>
       </c>
       <c r="N43">
-        <f t="shared" si="0"/>
-        <v>58</v>
+        <f t="shared" si="4"/>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2367,10 +2871,22 @@
       <c r="C44" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="6"/>
+      <c r="D44" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F44" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G44" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H44">
         <v>18</v>
       </c>
@@ -2384,7 +2900,7 @@
         <v>40</v>
       </c>
       <c r="N44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2398,10 +2914,22 @@
       <c r="C45" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="6"/>
+      <c r="D45" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F45" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
       <c r="H45">
         <v>17</v>
       </c>
@@ -2415,7 +2943,7 @@
         <v>40</v>
       </c>
       <c r="N45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
     </row>
@@ -2429,19 +2957,34 @@
       <c r="C46" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="6"/>
+      <c r="D46" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E46" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F46" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
       <c r="J46">
         <v>20</v>
       </c>
       <c r="K46">
         <v>1</v>
       </c>
+      <c r="L46">
+        <v>40</v>
+      </c>
       <c r="N46">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2454,10 +2997,22 @@
       <c r="C47" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="6"/>
+      <c r="D47" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E47" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F47" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G47" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H47">
         <v>18</v>
       </c>
@@ -2471,7 +3026,7 @@
         <v>35</v>
       </c>
       <c r="N47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2485,10 +3040,22 @@
       <c r="C48" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="6"/>
+      <c r="D48" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E48" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F48" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G48" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H48">
         <v>19</v>
       </c>
@@ -2502,7 +3069,7 @@
         <v>38</v>
       </c>
       <c r="N48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2516,10 +3083,22 @@
       <c r="C49" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="6"/>
+      <c r="D49" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E49" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G49" s="6">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
       <c r="H49">
         <v>10</v>
       </c>
@@ -2533,7 +3112,7 @@
         <v>30</v>
       </c>
       <c r="N49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
     </row>
@@ -2547,10 +3126,22 @@
       <c r="C50" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="6"/>
+      <c r="D50" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E50" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G50" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
       <c r="H50">
         <v>14</v>
       </c>
@@ -2564,7 +3155,7 @@
         <v>20</v>
       </c>
       <c r="N50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
     </row>
@@ -2578,10 +3169,22 @@
       <c r="C51" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="6"/>
+      <c r="D51" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E51" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F51" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G51" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J51">
         <v>10</v>
       </c>
@@ -2592,7 +3195,7 @@
         <v>40</v>
       </c>
       <c r="N51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
     </row>
@@ -2606,10 +3209,22 @@
       <c r="C52" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="6"/>
+      <c r="D52" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F52" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G52" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H52">
         <v>14</v>
       </c>
@@ -2623,7 +3238,7 @@
         <v>35</v>
       </c>
       <c r="N52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2637,10 +3252,25 @@
       <c r="C53" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="6"/>
+      <c r="D53" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F53" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G53" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>11</v>
+      </c>
       <c r="K53">
         <v>1</v>
       </c>
@@ -2648,8 +3278,8 @@
         <v>40</v>
       </c>
       <c r="N53">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f t="shared" si="4"/>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -2662,10 +3292,22 @@
       <c r="C54" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="6"/>
+      <c r="D54" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F54" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G54" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
       <c r="H54">
         <v>20</v>
       </c>
@@ -2679,7 +3321,7 @@
         <v>40</v>
       </c>
       <c r="N54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
     </row>
@@ -2693,10 +3335,22 @@
       <c r="C55" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="6"/>
+      <c r="D55" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F55" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G55" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
       <c r="H55">
         <v>19</v>
       </c>
@@ -2710,7 +3364,7 @@
         <v>30</v>
       </c>
       <c r="N55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
     </row>
@@ -2724,10 +3378,22 @@
       <c r="C56" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="6"/>
+      <c r="D56" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G56" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H56">
         <v>18</v>
       </c>
@@ -2741,7 +3407,7 @@
         <v>35</v>
       </c>
       <c r="N56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2755,10 +3421,22 @@
       <c r="C57" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="6"/>
+      <c r="D57" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E57" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F57" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G57" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="J57">
         <v>8</v>
       </c>
@@ -2769,7 +3447,7 @@
         <v>40</v>
       </c>
       <c r="N57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>48</v>
       </c>
     </row>
@@ -2783,10 +3461,22 @@
       <c r="C58" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="6"/>
+      <c r="D58" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F58" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G58" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H58">
         <v>17</v>
       </c>
@@ -2800,7 +3490,7 @@
         <v>40</v>
       </c>
       <c r="N58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2814,10 +3504,22 @@
       <c r="C59" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="6"/>
+      <c r="D59" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E59" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F59" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G59" s="6">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
       <c r="H59">
         <v>20</v>
       </c>
@@ -2831,7 +3533,7 @@
         <v>40</v>
       </c>
       <c r="N59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
     </row>
@@ -2845,10 +3547,22 @@
       <c r="C60" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="6"/>
+      <c r="D60" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E60" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F60" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G60" s="6">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
       <c r="H60">
         <v>14</v>
       </c>
@@ -2862,7 +3576,7 @@
         <v>35</v>
       </c>
       <c r="N60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>59</v>
       </c>
     </row>
@@ -2876,10 +3590,22 @@
       <c r="C61" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="6"/>
+      <c r="D61" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E61" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F61" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G61" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H61">
         <v>17</v>
       </c>
@@ -2893,7 +3619,7 @@
         <v>40</v>
       </c>
       <c r="N61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2907,10 +3633,22 @@
       <c r="C62" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="6"/>
+      <c r="D62" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E62" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F62" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G62" s="6">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
       <c r="H62">
         <v>17</v>
       </c>
@@ -2924,7 +3662,7 @@
         <v>40</v>
       </c>
       <c r="N62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
     </row>
@@ -2938,10 +3676,22 @@
       <c r="C63" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="6"/>
+      <c r="D63" s="6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E63" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="F63" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="G63" s="6">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
       <c r="H63">
         <v>18</v>
       </c>
@@ -2955,7 +3705,7 @@
         <v>35</v>
       </c>
       <c r="N63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
     </row>
@@ -2969,10 +3719,22 @@
       <c r="C64" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="6"/>
+      <c r="D64" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E64" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F64" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G64" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="H64">
         <v>10</v>
       </c>
@@ -2986,7 +3748,7 @@
         <v>20</v>
       </c>
       <c r="N64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
     </row>
@@ -3000,15 +3762,27 @@
       <c r="C65" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="6"/>
+      <c r="D65" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G65" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K65">
         <v>1</v>
       </c>
       <c r="N65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3022,15 +3796,27 @@
       <c r="C66" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="6"/>
+      <c r="D66" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E66" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F66" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G66" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="K66">
         <v>1</v>
       </c>
       <c r="N66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3044,15 +3830,27 @@
       <c r="C67" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="6"/>
+      <c r="D67" s="6" t="str">
+        <f t="shared" ref="D67:D83" si="5">IF((N67)&gt;=50,10,"")</f>
+        <v/>
+      </c>
+      <c r="E67" s="2" t="str">
+        <f t="shared" ref="E67:E83" si="6">IF((N67)&gt;=50,20,"")</f>
+        <v/>
+      </c>
+      <c r="F67" s="2" t="str">
+        <f t="shared" ref="F67:F83" si="7">IF((N67)&gt;=50,20,"")</f>
+        <v/>
+      </c>
+      <c r="G67" s="6" t="str">
+        <f t="shared" ref="G67:G83" si="8">IF((N67)&gt;=51,IF((N67-50)&gt;50,50,IF((N67-50)&lt;0,0,(N67-50))), "" )</f>
+        <v/>
+      </c>
       <c r="K67">
         <v>1</v>
       </c>
       <c r="N67">
-        <f t="shared" ref="N67:N83" si="1">IF((H67+J67+L67+M67+O67)&lt;70,IF((H67+J67+L67+M67+O67)&gt;64,70,(H67+J67+L67+M67+O67)),(H67+J67+L67+M67+O67))</f>
+        <f t="shared" ref="N67:N83" si="9">IF((H67+J67+L67+M67+O67)&lt;70,IF((H67+J67+L67+M67+O67)&gt;64,70,(H67+J67+L67+M67+O67)),(H67+J67+L67+M67+O67))</f>
         <v>0</v>
       </c>
     </row>
@@ -3066,15 +3864,27 @@
       <c r="C68" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="6"/>
+      <c r="D68" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E68" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F68" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G68" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="K68">
         <v>1</v>
       </c>
       <c r="N68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -3088,10 +3898,22 @@
       <c r="C69" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="6"/>
+      <c r="D69" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E69" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F69" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G69" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="H69">
         <v>16</v>
       </c>
@@ -3105,7 +3927,7 @@
         <v>20</v>
       </c>
       <c r="N69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
     </row>
@@ -3119,10 +3941,22 @@
       <c r="C70" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="6"/>
+      <c r="D70" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E70" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F70" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G70" s="6">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
       <c r="H70">
         <v>18</v>
       </c>
@@ -3136,7 +3970,7 @@
         <v>40</v>
       </c>
       <c r="N70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
     </row>
@@ -3150,10 +3984,22 @@
       <c r="C71" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="6"/>
+      <c r="D71" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E71" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F71" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G71" s="6">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
       <c r="J71">
         <v>20</v>
       </c>
@@ -3164,7 +4010,7 @@
         <v>35</v>
       </c>
       <c r="N71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
     </row>
@@ -3178,10 +4024,22 @@
       <c r="C72" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="D72" s="6"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="6"/>
+      <c r="D72" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E72" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F72" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G72" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="J72">
         <v>4</v>
       </c>
@@ -3192,7 +4050,7 @@
         <v>20</v>
       </c>
       <c r="N72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
     </row>
@@ -3206,10 +4064,22 @@
       <c r="C73" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="6"/>
+      <c r="D73" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E73" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F73" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G73" s="6">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
       <c r="H73">
         <v>16</v>
       </c>
@@ -3223,7 +4093,7 @@
         <v>40</v>
       </c>
       <c r="N73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
     </row>
@@ -3237,10 +4107,22 @@
       <c r="C74" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="6"/>
+      <c r="D74" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E74" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F74" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G74" s="6">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
       <c r="H74">
         <v>19</v>
       </c>
@@ -3254,7 +4136,7 @@
         <v>35</v>
       </c>
       <c r="N74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>74</v>
       </c>
     </row>
@@ -3268,10 +4150,22 @@
       <c r="C75" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="6"/>
+      <c r="D75" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E75" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F75" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G75" s="6">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
       <c r="H75">
         <v>16</v>
       </c>
@@ -3285,7 +4179,7 @@
         <v>40</v>
       </c>
       <c r="N75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>64</v>
       </c>
     </row>
@@ -3299,10 +4193,22 @@
       <c r="C76" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="6"/>
+      <c r="D76" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E76" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F76" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G76" s="6">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
       <c r="J76">
         <v>20</v>
       </c>
@@ -3313,7 +4219,7 @@
         <v>40</v>
       </c>
       <c r="N76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
     </row>
@@ -3327,10 +4233,22 @@
       <c r="C77" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D77" s="6"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="6"/>
+      <c r="D77" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E77" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F77" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G77" s="6">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
       <c r="H77">
         <v>19</v>
       </c>
@@ -3344,7 +4262,7 @@
         <v>40</v>
       </c>
       <c r="N77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
     </row>
@@ -3358,10 +4276,22 @@
       <c r="C78" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D78" s="6"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="6"/>
+      <c r="D78" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E78" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F78" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G78" s="6">
+        <f t="shared" si="8"/>
+        <v>28</v>
+      </c>
       <c r="H78">
         <v>18</v>
       </c>
@@ -3375,7 +4305,7 @@
         <v>40</v>
       </c>
       <c r="N78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>78</v>
       </c>
     </row>
@@ -3389,10 +4319,22 @@
       <c r="C79" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="D79" s="6"/>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="6"/>
+      <c r="D79" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E79" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F79" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G79" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="J79">
         <v>20</v>
       </c>
@@ -3403,7 +4345,7 @@
         <v>20</v>
       </c>
       <c r="N79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
     </row>
@@ -3417,10 +4359,22 @@
       <c r="C80" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="6"/>
+      <c r="D80" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E80" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F80" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G80" s="6">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
       <c r="H80">
         <v>16</v>
       </c>
@@ -3434,7 +4388,7 @@
         <v>30</v>
       </c>
       <c r="N80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
     </row>
@@ -3448,10 +4402,22 @@
       <c r="C81" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="D81" s="6"/>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="6"/>
+      <c r="D81" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E81" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F81" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G81" s="6">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
       <c r="H81">
         <v>10</v>
       </c>
@@ -3465,7 +4431,7 @@
         <v>40</v>
       </c>
       <c r="N81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>70</v>
       </c>
     </row>
@@ -3479,10 +4445,22 @@
       <c r="C82" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D82" s="6"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="6"/>
+      <c r="D82" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E82" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="F82" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="G82" s="6">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
       <c r="J82">
         <v>12</v>
       </c>
@@ -3493,7 +4471,7 @@
         <v>40</v>
       </c>
       <c r="N82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
         <v>52</v>
       </c>
     </row>
@@ -3507,13 +4485,28 @@
       <c r="C83" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="D83" s="6"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="6"/>
+      <c r="D83" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E83" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="F83" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="G83" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
       <c r="H83">
         <v>17</v>
       </c>
+      <c r="J83">
+        <v>11</v>
+      </c>
       <c r="K83">
         <v>1</v>
       </c>
@@ -3521,8 +4514,8 @@
         <v>20</v>
       </c>
       <c r="N83">
-        <f t="shared" si="1"/>
-        <v>37</v>
+        <f t="shared" si="9"/>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ya termine de todos, esta es la nota final que va a ser publicada, revisen y me dejan saber
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/BDatos.xlsx
+++ b/OYM/_DocumentosComunes/BDatos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_DESARROLLO\DocumentosUniversitarios\OYM\_DocumentosComunes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_DESARROLLO\DocumentosUniversitarios\OYM\_DocumentosComunes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C4AE384A-7E86-446C-92C6-43369297CEFF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page 1" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Page 1'!$A$1:$O$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Page 1'!$A$1:$G$83</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t>MATRICULA</t>
   </si>
@@ -557,12 +558,15 @@
   </si>
   <si>
     <t>JOSE  FRANCISCO DIAZ CORONA</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1097,18 +1101,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O83"/>
+  <dimension ref="A1:O89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -4629,8 +4633,13 @@
         <v>70</v>
       </c>
     </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O1">
+  <autoFilter ref="A1:O1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1" showButton="0"/>
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="3" showButton="0"/>

</xml_diff>